<commit_message>
Update test case Pelanggan, Salesman, Supplier
</commit_message>
<xml_diff>
--- a/Excel/DaftarBarang/BahanBakuDataExcel.xlsx
+++ b/Excel/DaftarBarang/BahanBakuDataExcel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6800"/>
+    <workbookView windowWidth="18350" windowHeight="6350"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>namabarang</t>
   </si>
@@ -78,6 +78,21 @@
   </si>
   <si>
     <t>Kodi</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>TEST1002</t>
+  </si>
+  <si>
+    <t>Gula Aren</t>
+  </si>
+  <si>
+    <t>Asd1fgh</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
 </sst>
 </file>
@@ -1233,13 +1248,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="4"/>
   <cols>
     <col min="1" max="1" width="12.3636363636364" customWidth="1"/>
     <col min="2" max="2" width="11.6363636363636" customWidth="1"/>
@@ -1321,6 +1336,46 @@
         <v>44</v>
       </c>
     </row>
+    <row r="3" spans="2:5">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add test case Bahan Kemas, Bahan Pembantu, Barang Setengah Jadi. Update Negative Case on Pelanggan.
</commit_message>
<xml_diff>
--- a/Excel/DaftarBarang/BahanBakuDataExcel.xlsx
+++ b/Excel/DaftarBarang/BahanBakuDataExcel.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>namabarang</t>
   </si>
@@ -71,7 +71,7 @@
     <t>Kilogram</t>
   </si>
   <si>
-    <t>Gula Pasir (edit)</t>
+    <t>Edited Sugar</t>
   </si>
   <si>
     <t>GP02</t>
@@ -80,19 +80,28 @@
     <t>Kodi</t>
   </si>
   <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>TEST1002</t>
-  </si>
-  <si>
-    <t>Gula Aren</t>
-  </si>
-  <si>
-    <t>Asd1fgh</t>
+    <t>Daun Teh</t>
+  </si>
+  <si>
+    <t>Qw2E0#</t>
+  </si>
+  <si>
+    <t>@!2000M</t>
+  </si>
+  <si>
+    <t>Kakao Bubuk</t>
+  </si>
+  <si>
+    <t>ASD</t>
   </si>
   <si>
     <t>TEST</t>
+  </si>
+  <si>
+    <t>Singkong</t>
+  </si>
+  <si>
+    <t>SK01</t>
   </si>
 </sst>
 </file>
@@ -708,8 +717,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1248,13 +1260,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="1" width="12.3636363636364" customWidth="1"/>
     <col min="2" max="2" width="11.6363636363636" customWidth="1"/>
@@ -1302,78 +1314,138 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>1000</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="2">
         <v>2</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="2">
         <v>1100</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
-      <c r="B3" t="s">
+    <row r="3" spans="1:11">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3"/>
-      <c r="E3">
-        <v>1001</v>
-      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+    <row r="4" spans="1:11">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
+      <c r="E4" s="2">
+        <v>1000</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5"/>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7">
+        <v>3000</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
-        <v>21</v>
+      <c r="J7" s="2">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>